<commit_message>
Pre-tx phase self report outcome measures added
</commit_message>
<xml_diff>
--- a/data/KAHI_brief_self.xlsx
+++ b/data/KAHI_brief_self.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jimwright/Desktop/University of Oregon Courses/Dissertation/Dissertation Clients/KAHI/participant_1_data/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C1606A0B-7964-7248-97B3-99605FE575F2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E17F49D-7024-8246-B90A-E97384233B3D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="32740" yWindow="2680" windowWidth="27640" windowHeight="15800" xr2:uid="{8AD1997E-D8CB-5944-A1E2-519BC3D1F2A2}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="27640" windowHeight="15800" xr2:uid="{8AD1997E-D8CB-5944-A1E2-519BC3D1F2A2}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -438,7 +438,7 @@
   <dimension ref="A1:D14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A13" sqref="A13"/>
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -470,6 +470,9 @@
       <c r="B2">
         <v>64</v>
       </c>
+      <c r="C2">
+        <v>64</v>
+      </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
@@ -478,6 +481,9 @@
       <c r="B3">
         <v>55</v>
       </c>
+      <c r="C3">
+        <v>55</v>
+      </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
@@ -486,6 +492,9 @@
       <c r="B4">
         <v>62</v>
       </c>
+      <c r="C4">
+        <v>62</v>
+      </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
@@ -494,6 +503,9 @@
       <c r="B5">
         <v>52</v>
       </c>
+      <c r="C5">
+        <v>58</v>
+      </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
@@ -502,6 +514,9 @@
       <c r="B6">
         <v>79</v>
       </c>
+      <c r="C6">
+        <v>82</v>
+      </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
@@ -510,6 +525,9 @@
       <c r="B7">
         <v>66</v>
       </c>
+      <c r="C7">
+        <v>71</v>
+      </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
@@ -523,6 +541,9 @@
       <c r="B9">
         <v>78</v>
       </c>
+      <c r="C9">
+        <v>78</v>
+      </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
@@ -531,6 +552,9 @@
       <c r="B10">
         <v>60</v>
       </c>
+      <c r="C10">
+        <v>66</v>
+      </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
@@ -539,6 +563,9 @@
       <c r="B11">
         <v>69</v>
       </c>
+      <c r="C11">
+        <v>75</v>
+      </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
@@ -552,6 +579,9 @@
       <c r="B13">
         <v>70</v>
       </c>
+      <c r="C13">
+        <v>74</v>
+      </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
@@ -559,6 +589,9 @@
       </c>
       <c r="B14">
         <v>68</v>
+      </c>
+      <c r="C14">
+        <v>72</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Final self-report BRIEF and CLASS responses added
</commit_message>
<xml_diff>
--- a/data/KAHI_brief_self.xlsx
+++ b/data/KAHI_brief_self.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11108"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11213"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jimwright/Desktop/University of Oregon Courses/Dissertation/Dissertation Clients/KAHI/participant_1_data/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6495A35-C0FB-E44F-848E-393B5104E8A7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AEE5ACEB-4B26-AC46-B0C8-57B5362FD809}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="27640" windowHeight="15800" xr2:uid="{8AD1997E-D8CB-5944-A1E2-519BC3D1F2A2}"/>
   </bookViews>
@@ -432,7 +432,7 @@
   <dimension ref="A1:D12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A20" sqref="A20"/>
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -467,6 +467,9 @@
       <c r="C2">
         <v>64</v>
       </c>
+      <c r="D2">
+        <v>67</v>
+      </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
@@ -478,6 +481,9 @@
       <c r="C3">
         <v>55</v>
       </c>
+      <c r="D3">
+        <v>46</v>
+      </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
@@ -489,6 +495,9 @@
       <c r="C4">
         <v>62</v>
       </c>
+      <c r="D4">
+        <v>59</v>
+      </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
@@ -500,6 +509,9 @@
       <c r="C5">
         <v>58</v>
       </c>
+      <c r="D5">
+        <v>71</v>
+      </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
@@ -511,6 +523,9 @@
       <c r="C6">
         <v>82</v>
       </c>
+      <c r="D6">
+        <v>79</v>
+      </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
@@ -522,6 +537,9 @@
       <c r="C7">
         <v>71</v>
       </c>
+      <c r="D7">
+        <v>77</v>
+      </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
@@ -533,6 +551,9 @@
       <c r="C8">
         <v>75</v>
       </c>
+      <c r="D8">
+        <v>86</v>
+      </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
@@ -544,6 +565,9 @@
       <c r="C9">
         <v>78</v>
       </c>
+      <c r="D9">
+        <v>82</v>
+      </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
@@ -555,6 +579,9 @@
       <c r="C10">
         <v>66</v>
       </c>
+      <c r="D10">
+        <v>63</v>
+      </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
@@ -566,6 +593,9 @@
       <c r="C11">
         <v>74</v>
       </c>
+      <c r="D11">
+        <v>78</v>
+      </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
@@ -576,6 +606,9 @@
       </c>
       <c r="C12">
         <v>72</v>
+      </c>
+      <c r="D12">
+        <v>75</v>
       </c>
     </row>
   </sheetData>

</xml_diff>